<commit_message>
style code distribution matrix
</commit_message>
<xml_diff>
--- a/doc/Distribution.xlsx
+++ b/doc/Distribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\FH\Master\grammAR\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\MCM\AR\grammAR\project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97939B0E-B2B8-4817-B8FF-C23AE4C062A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE83E81-359F-4547-880B-FD102180E2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25590" yWindow="0" windowWidth="12810" windowHeight="21000" xr2:uid="{28061F85-1A7D-4485-8DE6-5AF077E986B5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{28061F85-1A7D-4485-8DE6-5AF077E986B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
-    <t>Felix</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
     <t>ComponentConfig</t>
   </si>
   <si>
@@ -63,9 +56,6 @@
     <t>InfoBarTextBehaviour</t>
   </si>
   <si>
-    <t>LangButtonBehaviour</t>
-  </si>
-  <si>
     <t>SettingsTextBehaviour</t>
   </si>
   <si>
@@ -133,6 +123,15 @@
   </si>
   <si>
     <t>TextPosition</t>
+  </si>
+  <si>
+    <t>Felix Stumvoll</t>
+  </si>
+  <si>
+    <t>Manuel Fuchs</t>
+  </si>
+  <si>
+    <t>LanguageButtonBehaviour</t>
   </si>
 </sst>
 </file>
@@ -148,15 +147,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -164,12 +169,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,277 +546,282 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>119</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>164</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>94</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>92</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>17</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>14</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f>SUM(A2:A32)</f>
-        <v>609</v>
-      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
       <c r="B33">
         <f>SUM(B2:B32)</f>
+        <v>609</v>
+      </c>
+      <c r="C33">
+        <f>SUM(C2:C32)</f>
         <v>630</v>
       </c>
     </row>

</xml_diff>